<commit_message>
Evening of 4_10_2020 Storm 3.2
</commit_message>
<xml_diff>
--- a/LakeHodges/Storm 3/Hodges Creeks pacing worksheet_WW3.xlsx
+++ b/LakeHodges/Storm 3/Hodges Creeks pacing worksheet_WW3.xlsx
@@ -640,6 +640,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -649,6 +685,42 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -658,6 +730,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -666,87 +747,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,7 +785,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1191,7 +1191,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -1214,21 +1214,21 @@
       <c r="G2" s="24">
         <v>1000</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="44">
         <v>5000</v>
       </c>
-      <c r="I2" s="53">
+      <c r="I2" s="38">
         <v>1000</v>
       </c>
-      <c r="J2" s="56">
+      <c r="J2" s="41">
         <v>65</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="62" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1249,13 +1249,13 @@
       <c r="G3" s="26">
         <v>5000</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="42"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="63"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="25" t="s">
         <v>26</v>
       </c>
@@ -1276,13 +1276,13 @@
       <c r="G4" s="26">
         <v>8000</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="42"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="63"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="25" t="s">
         <v>7</v>
       </c>
@@ -1303,13 +1303,13 @@
       <c r="G5" s="26">
         <v>12000</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="42"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="63"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="25" t="s">
         <v>27</v>
       </c>
@@ -1330,13 +1330,13 @@
       <c r="G6" s="26">
         <v>16000</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="42"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="49"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
@@ -1357,13 +1357,13 @@
       <c r="G7" s="29">
         <v>19000</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="43"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="64"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -1386,21 +1386,21 @@
       <c r="G8" s="30">
         <v>4000</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="44">
         <v>20000</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="59">
+      <c r="J8" s="47">
         <v>63</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="62" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="25" t="s">
         <v>1</v>
       </c>
@@ -1421,13 +1421,13 @@
       <c r="G9" s="26">
         <v>13000</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="42"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="63"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="25" t="s">
         <v>26</v>
       </c>
@@ -1448,13 +1448,13 @@
       <c r="G10" s="26">
         <v>22000</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="42"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="63"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="25" t="s">
         <v>7</v>
       </c>
@@ -1475,13 +1475,13 @@
       <c r="G11" s="26">
         <v>30000</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="42"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="63"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="25" t="s">
         <v>27</v>
       </c>
@@ -1502,13 +1502,13 @@
       <c r="G12" s="26">
         <v>40000</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="42"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="63"/>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="49"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="27" t="s">
         <v>2</v>
       </c>
@@ -1529,13 +1529,13 @@
       <c r="G13" s="29">
         <v>48000</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="43"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="64"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="23" t="s">
@@ -1558,21 +1558,21 @@
       <c r="G14" s="30">
         <v>11000</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="44">
         <v>60000</v>
       </c>
       <c r="I14" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="35">
+      <c r="J14" s="59">
         <v>122</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="62" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="25" t="s">
         <v>1</v>
       </c>
@@ -1593,13 +1593,13 @@
       <c r="G15" s="26">
         <v>22000</v>
       </c>
-      <c r="H15" s="33"/>
+      <c r="H15" s="45"/>
       <c r="I15" s="51"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="42"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="63"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="48"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="25" t="s">
         <v>26</v>
       </c>
@@ -1620,13 +1620,13 @@
       <c r="G16" s="26">
         <v>33000</v>
       </c>
-      <c r="H16" s="33"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="51"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="42"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="63"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="25" t="s">
         <v>7</v>
       </c>
@@ -1647,13 +1647,13 @@
       <c r="G17" s="26">
         <v>44000</v>
       </c>
-      <c r="H17" s="33"/>
+      <c r="H17" s="45"/>
       <c r="I17" s="51"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="42"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="63"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="25" t="s">
         <v>27</v>
       </c>
@@ -1674,13 +1674,13 @@
       <c r="G18" s="26">
         <v>54000</v>
       </c>
-      <c r="H18" s="33"/>
+      <c r="H18" s="45"/>
       <c r="I18" s="51"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="42"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="63"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="49"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="27" t="s">
         <v>2</v>
       </c>
@@ -1701,13 +1701,13 @@
       <c r="G19" s="29">
         <v>65000</v>
       </c>
-      <c r="H19" s="34"/>
+      <c r="H19" s="46"/>
       <c r="I19" s="52"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="43"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="64"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="23" t="s">
@@ -1730,21 +1730,21 @@
       <c r="G20" s="30">
         <v>2000</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="44">
         <v>30000</v>
       </c>
-      <c r="I20" s="62" t="s">
+      <c r="I20" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="J20" s="65" t="s">
+      <c r="J20" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="62" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
@@ -1765,13 +1765,13 @@
       <c r="G21" s="26">
         <v>15000</v>
       </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="42"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="63"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="25" t="s">
         <v>26</v>
       </c>
@@ -1792,13 +1792,13 @@
       <c r="G22" s="26">
         <v>45000</v>
       </c>
-      <c r="H22" s="33"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="42"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="63"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="25" t="s">
         <v>7</v>
       </c>
@@ -1819,13 +1819,13 @@
       <c r="G23" s="26">
         <v>97000</v>
       </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="42"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="25" t="s">
         <v>27</v>
       </c>
@@ -1846,13 +1846,13 @@
       <c r="G24" s="26">
         <v>136000</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="42"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="63"/>
     </row>
     <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="49"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="27" t="s">
         <v>2</v>
       </c>
@@ -1873,13 +1873,13 @@
       <c r="G25" s="29">
         <v>170000</v>
       </c>
-      <c r="H25" s="34"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="43"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="64"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="23" t="s">
@@ -1902,21 +1902,21 @@
       <c r="G26" s="30">
         <v>13000</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="44">
         <v>50000</v>
       </c>
-      <c r="I26" s="62">
+      <c r="I26" s="53">
         <v>30000</v>
       </c>
-      <c r="J26" s="65">
+      <c r="J26" s="56">
         <v>40</v>
       </c>
-      <c r="K26" s="41" t="s">
+      <c r="K26" s="62" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="48"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="25" t="s">
         <v>1</v>
       </c>
@@ -1937,13 +1937,13 @@
       <c r="G27" s="26">
         <v>33000</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="42"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="63"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="48"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="25" t="s">
         <v>26</v>
       </c>
@@ -1964,13 +1964,13 @@
       <c r="G28" s="26">
         <v>52000</v>
       </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="42"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="63"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="48"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="25" t="s">
         <v>7</v>
       </c>
@@ -1991,13 +1991,13 @@
       <c r="G29" s="26">
         <v>71000</v>
       </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="42"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="63"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="25" t="s">
         <v>27</v>
       </c>
@@ -2018,13 +2018,13 @@
       <c r="G30" s="26">
         <v>91000</v>
       </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="42"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="63"/>
     </row>
     <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="49"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="27" t="s">
         <v>2</v>
       </c>
@@ -2045,13 +2045,13 @@
       <c r="G31" s="29">
         <v>110000</v>
       </c>
-      <c r="H31" s="34"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="43"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="64"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="35" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="23" t="s">
@@ -2074,21 +2074,21 @@
       <c r="G32" s="30">
         <v>38000</v>
       </c>
-      <c r="H32" s="32">
+      <c r="H32" s="44">
         <v>45000</v>
       </c>
-      <c r="I32" s="62">
+      <c r="I32" s="53">
         <v>40000</v>
       </c>
-      <c r="J32" s="65">
+      <c r="J32" s="56">
         <v>60</v>
       </c>
-      <c r="K32" s="41" t="s">
+      <c r="K32" s="62" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="25" t="s">
         <v>1</v>
       </c>
@@ -2109,13 +2109,13 @@
       <c r="G33" s="26">
         <v>44000</v>
       </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="42"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="63"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="25" t="s">
         <v>26</v>
       </c>
@@ -2136,13 +2136,13 @@
       <c r="G34" s="26">
         <v>49000</v>
       </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="42"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="63"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="25" t="s">
         <v>7</v>
       </c>
@@ -2163,13 +2163,13 @@
       <c r="G35" s="26">
         <v>55000</v>
       </c>
-      <c r="H35" s="33"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="42"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="63"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="25" t="s">
         <v>27</v>
       </c>
@@ -2190,13 +2190,13 @@
       <c r="G36" s="26">
         <v>61000</v>
       </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="42"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="63"/>
     </row>
     <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="46"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="27" t="s">
         <v>2</v>
       </c>
@@ -2217,13 +2217,13 @@
       <c r="G37" s="29">
         <v>67000</v>
       </c>
-      <c r="H37" s="34"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="67"/>
-      <c r="K37" s="43"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="64"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="23" t="s">
@@ -2246,21 +2246,21 @@
       <c r="G38" s="30">
         <v>5000</v>
       </c>
-      <c r="H38" s="38">
+      <c r="H38" s="65">
         <v>100000</v>
       </c>
       <c r="I38" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="J38" s="35">
+      <c r="J38" s="59">
         <v>132</v>
       </c>
-      <c r="K38" s="41" t="s">
+      <c r="K38" s="62" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="25" t="s">
         <v>1</v>
       </c>
@@ -2281,13 +2281,13 @@
       <c r="G39" s="26">
         <v>12000</v>
       </c>
-      <c r="H39" s="39"/>
+      <c r="H39" s="66"/>
       <c r="I39" s="51"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="42"/>
+      <c r="J39" s="60"/>
+      <c r="K39" s="63"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="A40" s="36"/>
       <c r="B40" s="25" t="s">
         <v>26</v>
       </c>
@@ -2308,13 +2308,13 @@
       <c r="G40" s="26">
         <v>19000</v>
       </c>
-      <c r="H40" s="39"/>
+      <c r="H40" s="66"/>
       <c r="I40" s="51"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="42"/>
+      <c r="J40" s="60"/>
+      <c r="K40" s="63"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="A41" s="36"/>
       <c r="B41" s="25" t="s">
         <v>7</v>
       </c>
@@ -2335,13 +2335,13 @@
       <c r="G41" s="26">
         <v>26000</v>
       </c>
-      <c r="H41" s="39"/>
+      <c r="H41" s="66"/>
       <c r="I41" s="51"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="42"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="63"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="25" t="s">
         <v>27</v>
       </c>
@@ -2362,13 +2362,13 @@
       <c r="G42" s="26">
         <v>33000</v>
       </c>
-      <c r="H42" s="39"/>
+      <c r="H42" s="66"/>
       <c r="I42" s="51"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="42"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="63"/>
     </row>
     <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="46"/>
+      <c r="A43" s="37"/>
       <c r="B43" s="27" t="s">
         <v>2</v>
       </c>
@@ -2389,13 +2389,13 @@
       <c r="G43" s="29">
         <v>40000</v>
       </c>
-      <c r="H43" s="40"/>
+      <c r="H43" s="67"/>
       <c r="I43" s="52"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="43"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="64"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="32" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="23" t="s">
@@ -2418,21 +2418,21 @@
       <c r="G44" s="30">
         <v>12000</v>
       </c>
-      <c r="H44" s="32">
+      <c r="H44" s="44">
         <v>2000</v>
       </c>
       <c r="I44" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="J44" s="35">
+      <c r="J44" s="59">
         <v>0</v>
       </c>
-      <c r="K44" s="41" t="s">
+      <c r="K44" s="62" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="48"/>
+      <c r="A45" s="33"/>
       <c r="B45" s="25" t="s">
         <v>1</v>
       </c>
@@ -2453,13 +2453,13 @@
       <c r="G45" s="26">
         <v>65000</v>
       </c>
-      <c r="H45" s="33"/>
+      <c r="H45" s="45"/>
       <c r="I45" s="51"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="42"/>
+      <c r="J45" s="60"/>
+      <c r="K45" s="63"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="48"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="25" t="s">
         <v>26</v>
       </c>
@@ -2480,13 +2480,13 @@
       <c r="G46" s="26">
         <v>118000</v>
       </c>
-      <c r="H46" s="33"/>
+      <c r="H46" s="45"/>
       <c r="I46" s="51"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="42"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="63"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="48"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="25" t="s">
         <v>7</v>
       </c>
@@ -2507,13 +2507,13 @@
       <c r="G47" s="26">
         <v>170000</v>
       </c>
-      <c r="H47" s="33"/>
+      <c r="H47" s="45"/>
       <c r="I47" s="51"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="42"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="63"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="48"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="25" t="s">
         <v>27</v>
       </c>
@@ -2534,13 +2534,13 @@
       <c r="G48" s="26">
         <v>223000</v>
       </c>
-      <c r="H48" s="33"/>
+      <c r="H48" s="45"/>
       <c r="I48" s="51"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="42"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="63"/>
     </row>
     <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="49"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="27" t="s">
         <v>2</v>
       </c>
@@ -2561,13 +2561,13 @@
       <c r="G49" s="29">
         <v>274000</v>
       </c>
-      <c r="H49" s="34"/>
+      <c r="H49" s="46"/>
       <c r="I49" s="52"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="43"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="64"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="32" t="s">
         <v>13</v>
       </c>
       <c r="B50" s="23" t="s">
@@ -2590,21 +2590,21 @@
       <c r="G50" s="30">
         <v>2600</v>
       </c>
-      <c r="H50" s="32">
+      <c r="H50" s="44">
         <v>8000</v>
       </c>
       <c r="I50" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="J50" s="35">
+      <c r="J50" s="59">
         <v>145</v>
       </c>
-      <c r="K50" s="41" t="s">
+      <c r="K50" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="48"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="25" t="s">
         <v>1</v>
       </c>
@@ -2625,13 +2625,13 @@
       <c r="G51" s="26">
         <v>14000</v>
       </c>
-      <c r="H51" s="33"/>
+      <c r="H51" s="45"/>
       <c r="I51" s="51"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="42"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="63"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="48"/>
+      <c r="A52" s="33"/>
       <c r="B52" s="25" t="s">
         <v>26</v>
       </c>
@@ -2652,13 +2652,13 @@
       <c r="G52" s="26">
         <v>25000</v>
       </c>
-      <c r="H52" s="33"/>
+      <c r="H52" s="45"/>
       <c r="I52" s="51"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="42"/>
+      <c r="J52" s="60"/>
+      <c r="K52" s="63"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="48"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="25" t="s">
         <v>7</v>
       </c>
@@ -2679,13 +2679,13 @@
       <c r="G53" s="26">
         <v>36000</v>
       </c>
-      <c r="H53" s="33"/>
+      <c r="H53" s="45"/>
       <c r="I53" s="51"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="42"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="63"/>
     </row>
     <row r="54" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="48"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="25" t="s">
         <v>27</v>
       </c>
@@ -2706,13 +2706,13 @@
       <c r="G54" s="26">
         <v>46000</v>
       </c>
-      <c r="H54" s="33"/>
+      <c r="H54" s="45"/>
       <c r="I54" s="51"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="42"/>
+      <c r="J54" s="60"/>
+      <c r="K54" s="63"/>
     </row>
     <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="49"/>
+      <c r="A55" s="34"/>
       <c r="B55" s="27" t="s">
         <v>2</v>
       </c>
@@ -2733,10 +2733,10 @@
       <c r="G55" s="29">
         <v>60000</v>
       </c>
-      <c r="H55" s="34"/>
+      <c r="H55" s="46"/>
       <c r="I55" s="52"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="43"/>
+      <c r="J55" s="61"/>
+      <c r="K55" s="64"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -2745,11 +2745,30 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="H14:H19"/>
+    <mergeCell ref="H20:H25"/>
+    <mergeCell ref="J38:J43"/>
+    <mergeCell ref="H38:H43"/>
+    <mergeCell ref="K32:K37"/>
+    <mergeCell ref="K38:K43"/>
+    <mergeCell ref="K44:K49"/>
+    <mergeCell ref="K50:K55"/>
+    <mergeCell ref="J14:J19"/>
+    <mergeCell ref="K2:K7"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="K14:K19"/>
+    <mergeCell ref="K20:K25"/>
+    <mergeCell ref="K26:K31"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="J44:J49"/>
+    <mergeCell ref="H44:H49"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="I38:I43"/>
+    <mergeCell ref="I44:I49"/>
+    <mergeCell ref="I50:I55"/>
+    <mergeCell ref="J50:J55"/>
+    <mergeCell ref="H50:H55"/>
     <mergeCell ref="A32:A37"/>
     <mergeCell ref="I2:I7"/>
     <mergeCell ref="J2:J7"/>
@@ -2766,30 +2785,11 @@
     <mergeCell ref="H26:H31"/>
     <mergeCell ref="J32:J37"/>
     <mergeCell ref="H32:H37"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="J44:J49"/>
-    <mergeCell ref="H44:H49"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="I38:I43"/>
-    <mergeCell ref="I44:I49"/>
-    <mergeCell ref="I50:I55"/>
-    <mergeCell ref="J50:J55"/>
-    <mergeCell ref="H50:H55"/>
-    <mergeCell ref="K44:K49"/>
-    <mergeCell ref="K50:K55"/>
-    <mergeCell ref="J14:J19"/>
-    <mergeCell ref="K2:K7"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="K14:K19"/>
-    <mergeCell ref="K20:K25"/>
-    <mergeCell ref="K26:K31"/>
-    <mergeCell ref="H14:H19"/>
-    <mergeCell ref="H20:H25"/>
-    <mergeCell ref="J38:J43"/>
-    <mergeCell ref="H38:H43"/>
-    <mergeCell ref="K32:K37"/>
-    <mergeCell ref="K38:K43"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="portrait" r:id="rId1"/>

</xml_diff>